<commit_message>
atualização controle do fluxo dos processos
</commit_message>
<xml_diff>
--- a/database/controle_processos_novo.xlsx
+++ b/database/controle_processos_novo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/63fbdbda17b5124d/Área de Trabalho/Programa git/pyqt6/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb5bd7a50d11ebd7/Área de Trabalho/Programa PYQT6/pyqt6/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{3F9171CD-0CBE-47B7-85D1-F497B68483DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB9F16EC-4618-4B08-B978-AC4D4717AA2A}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{3F9171CD-0CBE-47B7-85D1-F497B68483DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1ECE1F9F-89F8-4E61-A3C7-CD36BE909FFC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,9 +61,6 @@
     <t>Material Escolar</t>
   </si>
   <si>
-    <t>modalidade</t>
-  </si>
-  <si>
     <t>CC 01/2024</t>
   </si>
   <si>
@@ -83,6 +80,9 @@
   </si>
   <si>
     <t>PE 13/2023</t>
+  </si>
+  <si>
+    <t>id_processo</t>
   </si>
 </sst>
 </file>
@@ -461,24 +461,24 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.08984375" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="32.6640625" customWidth="1"/>
+    <col min="3" max="3" width="32.6328125" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -499,57 +499,57 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>

</xml_diff>